<commit_message>
FIX: Control library updates
</commit_message>
<xml_diff>
--- a/Curves/class8_truck_AccelCurve.xlsx
+++ b/Curves/class8_truck_AccelCurve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\OneDrive\Documents\MATLAB\Crash_Simulator\CrashSimulator\LimitCurves\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\codex\w\SafetyVehicleSimulator\Curves\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6881CD20-70A3-4544-8527-2EBA88F776E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F27A3F-791A-467F-9949-794B2CA7B656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="86303" yWindow="-98" windowWidth="28995" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
@@ -1336,12 +1336,12 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,15 +1349,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>0.75</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1.25</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1.75</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>2.5</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3.5</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>12</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>13</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>14</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>15</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>17</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>18</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>20</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>21</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>22</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>23</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>24</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>25</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>26</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>27</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>28</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>29</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>30</v>
       </c>

</xml_diff>